<commit_message>
almost completed corporate master
</commit_message>
<xml_diff>
--- a/public/Sample_Folios.xlsx
+++ b/public/Sample_Folios.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>Equity Type</t>
+  </si>
   <si>
     <t>Folio</t>
   </si>
@@ -1264,14 +1267,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="13" width="12.6719" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.6719" style="1" customWidth="1"/>
+    <col min="1" max="14" width="12.6719" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1314,21 +1317,25 @@
       <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
+      <c r="N1" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
       <c r="A3" s="6"/>
@@ -1344,6 +1351,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
       <c r="A4" s="7"/>
@@ -1359,6 +1367,7 @@
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
       <c r="A5" s="7"/>
@@ -1374,6 +1383,7 @@
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" s="7"/>
@@ -1389,6 +1399,7 @@
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" s="7"/>
@@ -1404,6 +1415,7 @@
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
       <c r="A8" s="7"/>
@@ -1419,6 +1431,7 @@
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
       <c r="A9" s="7"/>
@@ -1434,6 +1447,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="7"/>
@@ -1449,6 +1463,7 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>